<commit_message>
Loan customer also mail sent
</commit_message>
<xml_diff>
--- a/Input Files/LoanData_Modified.xlsx
+++ b/Input Files/LoanData_Modified.xlsx
@@ -330,7 +330,7 @@
     <x:t>Raubach</x:t>
   </x:si>
   <x:si>
-    <x:t>Successfully applied for the loan. Account Number: 6513e787158a51004651b63c</x:t>
+    <x:t>Successfully applied for the loan. Account Number: 6513fa7b158a51004651b66e</x:t>
   </x:si>
   <x:si>
     <x:t>Ethel</x:t>
@@ -345,7 +345,7 @@
     <x:t>Hergatz</x:t>
   </x:si>
   <x:si>
-    <x:t>Successfully applied for the loan. Account Number: 6513e7a4158a51004651b63d</x:t>
+    <x:t>Successfully applied for the loan. Account Number: 6513fa9b158a51004651b66f</x:t>
   </x:si>
   <x:si>
     <x:t>Jeremy</x:t>
@@ -360,7 +360,7 @@
     <x:t>Nürnberg</x:t>
   </x:si>
   <x:si>
-    <x:t>Successfully applied for the loan. Account Number: 6513e7bf158a51004651b63e</x:t>
+    <x:t>Successfully applied for the loan. Account Number: 6513fab8158a51004651b670</x:t>
   </x:si>
   <x:si>
     <x:t>Bethany</x:t>
@@ -480,7 +480,7 @@
     <x:t>Hamburg Billstedt</x:t>
   </x:si>
   <x:si>
-    <x:t>Successfully applied for the loan. Account Number: 6513e7db158a51004651b63f</x:t>
+    <x:t>Successfully applied for the loan. Account Number: 6513fad6158a51004651b671</x:t>
   </x:si>
   <x:si>
     <x:t>Jeffery</x:t>
@@ -495,7 +495,7 @@
     <x:t>Albersdorf</x:t>
   </x:si>
   <x:si>
-    <x:t>Successfully applied for the loan. Account Number: 6513e7f5158a51004651b640</x:t>
+    <x:t>Successfully applied for the loan. Account Number: 6513faf6158a51004651b672</x:t>
   </x:si>
   <x:si>
     <x:t>Katrina</x:t>

</xml_diff>